<commit_message>
Se agrega la funcionalidad de ´Olvide mi contraseña´ y se agregan comentarios
</commit_message>
<xml_diff>
--- a/Dashboards/Analisis_Maqueta_Sistema_Solar.xlsx
+++ b/Dashboards/Analisis_Maqueta_Sistema_Solar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f6cef8f20efdf97/Escritorio/UNIVERSIDAD/ALGORITMOS/SistemaSolarSTEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f6cef8f20efdf97/Escritorio/UNIVERSIDAD/ALGORITMOS/SistemaSolarSTEM/Sistema_Solar_STEM/Dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{5B957774-B922-4293-A708-42CBC1D75859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{792D52AC-C55B-4560-8D27-00CB8C141140}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="13_ncr:1_{5B957774-B922-4293-A708-42CBC1D75859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8CC167F-7B31-4337-A2C4-D121F5621F3F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="78">
   <si>
     <t>Escenario</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Presupuesto</t>
+  </si>
+  <si>
+    <t>Cinta de Aislar</t>
+  </si>
+  <si>
+    <t>Estrellitas</t>
   </si>
 </sst>
 </file>
@@ -593,8 +599,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40A4B4DE-B559-4B91-9751-FAEBFB93A291}" name="Tabla2" displayName="Tabla2" ref="A1:F21" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A1:F21" xr:uid="{40A4B4DE-B559-4B91-9751-FAEBFB93A291}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40A4B4DE-B559-4B91-9751-FAEBFB93A291}" name="Tabla2" displayName="Tabla2" ref="A1:F23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:F23" xr:uid="{40A4B4DE-B559-4B91-9751-FAEBFB93A291}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E52A7749-4176-4C6A-947B-991340A8755E}" name="Componente" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{A5E89885-A9DD-463B-B34E-79D6E390FA83}" name="Unidad" dataDxfId="4"/>
@@ -1397,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77BF8EC-75D8-4F8F-A926-3B2EF81C70D0}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1450,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="9">
         <v>299</v>
@@ -1454,11 +1460,11 @@
       </c>
       <c r="E2" s="9">
         <f>Tabla2[[#This Row],[Costo]]*Tabla2[[#This Row],[Unidad]]</f>
-        <v>299</v>
+        <v>598</v>
       </c>
       <c r="F2" s="9">
         <f>$H$2-Tabla2[[#This Row],[Total]]</f>
-        <v>951</v>
+        <v>652</v>
       </c>
       <c r="H2" s="13">
         <v>1250</v>
@@ -1483,7 +1489,7 @@
       </c>
       <c r="F3" s="9">
         <f>F2-Tabla2[[#This Row],[Total]]</f>
-        <v>812</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1505,7 +1511,7 @@
       </c>
       <c r="F4" s="9">
         <f>F3-Tabla2[[#This Row],[Total]]</f>
-        <v>692</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1527,7 +1533,7 @@
       </c>
       <c r="F5" s="9">
         <f>F4-Tabla2[[#This Row],[Total]]</f>
-        <v>692</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1549,7 +1555,7 @@
       </c>
       <c r="F6" s="9">
         <f>F5-Tabla2[[#This Row],[Total]]</f>
-        <v>655.5</v>
+        <v>356.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1571,7 +1577,7 @@
       </c>
       <c r="F7" s="9">
         <f>F6-Tabla2[[#This Row],[Total]]</f>
-        <v>576.5</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,7 +1599,7 @@
       </c>
       <c r="F8" s="9">
         <f>F7-Tabla2[[#This Row],[Total]]</f>
-        <v>576.5</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1615,7 +1621,7 @@
       </c>
       <c r="F9" s="9">
         <f>F8-Tabla2[[#This Row],[Total]]</f>
-        <v>576.5</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,7 +1643,7 @@
       </c>
       <c r="F10" s="9">
         <f>F9-Tabla2[[#This Row],[Total]]</f>
-        <v>575.9</v>
+        <v>276.89999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1659,7 +1665,7 @@
       </c>
       <c r="F11" s="9">
         <f>F10-Tabla2[[#This Row],[Total]]</f>
-        <v>573.9</v>
+        <v>274.89999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1681,7 +1687,7 @@
       </c>
       <c r="F12" s="9">
         <f>F11-Tabla2[[#This Row],[Total]]</f>
-        <v>571.6</v>
+        <v>272.59999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1703,7 +1709,7 @@
       </c>
       <c r="F13" s="9">
         <f>F12-Tabla2[[#This Row],[Total]]</f>
-        <v>566.80000000000007</v>
+        <v>267.79999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1725,7 +1731,7 @@
       </c>
       <c r="F14" s="9">
         <f>F13-Tabla2[[#This Row],[Total]]</f>
-        <v>563.55000000000007</v>
+        <v>264.54999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,7 +1753,7 @@
       </c>
       <c r="F15" s="9">
         <f>F14-Tabla2[[#This Row],[Total]]</f>
-        <v>558.45000000000005</v>
+        <v>259.44999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1769,7 +1775,7 @@
       </c>
       <c r="F16" s="9">
         <f>F15-Tabla2[[#This Row],[Total]]</f>
-        <v>550.85</v>
+        <v>251.84999999999994</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1791,7 +1797,7 @@
       </c>
       <c r="F17" s="9">
         <f>F16-Tabla2[[#This Row],[Total]]</f>
-        <v>547.70000000000005</v>
+        <v>248.69999999999993</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1813,7 +1819,7 @@
       </c>
       <c r="F18" s="9">
         <f>F17-Tabla2[[#This Row],[Total]]</f>
-        <v>544.35</v>
+        <v>245.34999999999994</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1835,7 +1841,7 @@
       </c>
       <c r="F19" s="9">
         <f>F18-Tabla2[[#This Row],[Total]]</f>
-        <v>532.6</v>
+        <v>233.59999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,7 +1863,7 @@
       </c>
       <c r="F20" s="9">
         <f>F19-Tabla2[[#This Row],[Total]]</f>
-        <v>514.15</v>
+        <v>215.14999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1879,7 +1885,51 @@
       </c>
       <c r="F21" s="9">
         <f>F20-Tabla2[[#This Row],[Total]]</f>
-        <v>504.59999999999997</v>
+        <v>205.59999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>10</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="9">
+        <f>Tabla2[[#This Row],[Costo]]*Tabla2[[#This Row],[Unidad]]</f>
+        <v>10</v>
+      </c>
+      <c r="F22" s="9">
+        <f>F21-Tabla2[[#This Row],[Total]]</f>
+        <v>195.59999999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="9">
+        <f>Tabla2[[#This Row],[Costo]]*Tabla2[[#This Row],[Unidad]]</f>
+        <v>3.5</v>
+      </c>
+      <c r="F23" s="9">
+        <f>F22-Tabla2[[#This Row],[Total]]</f>
+        <v>192.09999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>